<commit_message>
added categories, axis titles, and chart title to line chart in excel
</commit_message>
<xml_diff>
--- a/RealPython/openpyxl/xl_line_chart.xlsx
+++ b/RealPython/openpyxl/xl_line_chart.xlsx
@@ -127,6 +127,21 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Sales per month</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
     <plotArea>
       <lineChart>
         <grouping val="standard"/>
@@ -151,6 +166,11 @@
               </a:ln>
             </spPr>
           </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$1:$M$1</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
               <f>'Sheet'!$B$2:$M$2</f>
@@ -178,6 +198,11 @@
               </a:ln>
             </spPr>
           </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$1:$M$1</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
               <f>'Sheet'!$B$3:$M$3</f>
@@ -205,6 +230,11 @@
               </a:ln>
             </spPr>
           </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$1:$M$1</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
               <f>'Sheet'!$B$4:$M$4</f>
@@ -220,6 +250,21 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -232,6 +277,21 @@
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sales</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="10"/>
@@ -638,40 +698,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C2" t="n">
+        <v>63</v>
+      </c>
+      <c r="D2" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>99</v>
+      </c>
+      <c r="G2" t="n">
+        <v>79</v>
+      </c>
+      <c r="H2" t="n">
         <v>50</v>
       </c>
-      <c r="C2" t="n">
-        <v>53</v>
-      </c>
-      <c r="D2" t="n">
-        <v>22</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17</v>
-      </c>
-      <c r="F2" t="n">
-        <v>74</v>
-      </c>
-      <c r="G2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2" t="n">
-        <v>98</v>
-      </c>
       <c r="I2" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="J2" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="K2" t="n">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="L2" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="M2" t="n">
-        <v>82</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -679,40 +739,40 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>21</v>
+      </c>
+      <c r="C3" t="n">
+        <v>97</v>
+      </c>
+      <c r="D3" t="n">
+        <v>81</v>
+      </c>
+      <c r="E3" t="n">
+        <v>52</v>
+      </c>
+      <c r="F3" t="n">
         <v>40</v>
       </c>
-      <c r="C3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>93</v>
-      </c>
-      <c r="E3" t="n">
-        <v>30</v>
-      </c>
-      <c r="F3" t="n">
-        <v>8</v>
-      </c>
       <c r="G3" t="n">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="H3" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="I3" t="n">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="J3" t="n">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="K3" t="n">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="L3" t="n">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="M3" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
@@ -720,40 +780,40 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C4" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D4" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="F4" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G4" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="H4" t="n">
         <v>91</v>
       </c>
       <c r="I4" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="J4" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="K4" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" t="n">
         <v>64</v>
       </c>
-      <c r="L4" t="n">
-        <v>18</v>
-      </c>
       <c r="M4" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>